<commit_message>
Ajuste a los estados mensuales y migracion
</commit_message>
<xml_diff>
--- a/migracion/migracionXnit.xlsx
+++ b/migracion/migracionXnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\DesarrolloWeb358\gestion-global\migracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E519B4A-3BDE-4FF6-8AB4-7F3D7D3714F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882E9984-EC53-419D-990D-7CBB37B26583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{23831529-313D-4FD4-9556-5C5894147868}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>nit</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>3zTvYdP34DT0BJWIQnCMD1xRN3l1</t>
+  </si>
+  <si>
+    <t>conjunto residencial porvenir reservado casas 2</t>
   </si>
 </sst>
 </file>
@@ -436,7 +439,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
@@ -527,7 +530,12 @@
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="B8" s="1"/>
+      <c r="A8" s="1">
+        <v>900242908</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>

</xml_diff>

<commit_message>
ajuste en la migracion de los procesos judiciales para el cliente
</commit_message>
<xml_diff>
--- a/migracion/migracionXnit.xlsx
+++ b/migracion/migracionXnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\DesarrolloWeb358\gestion-global\migracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DCF0B6-99AD-4BCE-A9D5-985D7E44C59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7A137A-AF06-4966-BE0C-C71F14336C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{23831529-313D-4FD4-9556-5C5894147868}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,33 +50,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,13 +65,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -123,16 +97,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57688D05-55A1-47BC-8BE5-91F4BB88B5A9}">
-  <dimension ref="A1:D107"/>
+  <dimension ref="A1:A60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
@@ -460,377 +431,309 @@
     <col min="3" max="3" width="30.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A2" s="5">
-        <v>800142993</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A3" s="5">
-        <v>800177027</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A4" s="5">
-        <v>800184481</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A5" s="5">
-        <v>800193176</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A6" s="6">
-        <v>800198168</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A7" s="6">
-        <v>800206093</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A8" s="6">
-        <v>800217483</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
-        <v>800234376</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
-        <v>800237079</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
-        <v>809011754</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="6">
-        <v>830002298</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="6">
-        <v>830015808</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="4"/>
+    <row r="2" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>830035457</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>830047278</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>830057747</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>830071809</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>830074497</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2">
+        <v>830075332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="3">
+        <v>900687420</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="3">
+        <v>900346849</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="3">
+        <v>900281120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="3">
+        <v>900003261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="3">
+        <v>900947384</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="3">
+        <v>901507077</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="3">
+        <v>900719501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="3">
+        <v>900658412</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="3">
+        <v>900182882</v>
+      </c>
     </row>
     <row r="17" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="4"/>
+      <c r="A17" s="3">
+        <v>900061167</v>
+      </c>
     </row>
     <row r="18" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="4"/>
+      <c r="A18" s="3">
+        <v>901001861</v>
+      </c>
     </row>
     <row r="19" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="4"/>
+      <c r="A19" s="3">
+        <v>900123743</v>
+      </c>
     </row>
     <row r="20" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="4"/>
+      <c r="A20" s="3">
+        <v>900377532</v>
+      </c>
     </row>
     <row r="21" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="4"/>
+      <c r="A21" s="3">
+        <v>900190116</v>
+      </c>
     </row>
     <row r="22" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="4"/>
+      <c r="A22" s="3">
+        <v>900155802</v>
+      </c>
     </row>
     <row r="23" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="4"/>
+      <c r="A23" s="3">
+        <v>900506434</v>
+      </c>
     </row>
     <row r="24" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="4"/>
+      <c r="A24" s="3">
+        <v>830121765</v>
+      </c>
     </row>
     <row r="25" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="4"/>
+      <c r="A25" s="3">
+        <v>900122253</v>
+      </c>
     </row>
     <row r="26" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="4"/>
+      <c r="A26" s="3">
+        <v>830096405</v>
+      </c>
     </row>
     <row r="27" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="4"/>
+      <c r="A27" s="3">
+        <v>860040335</v>
+      </c>
     </row>
     <row r="28" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="4"/>
+      <c r="A28" s="3">
+        <v>901194167</v>
+      </c>
     </row>
     <row r="29" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="4"/>
+      <c r="A29" s="3">
+        <v>901132823</v>
+      </c>
     </row>
     <row r="30" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="4"/>
+      <c r="A30" s="3">
+        <v>830125131</v>
+      </c>
     </row>
     <row r="31" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="4"/>
+      <c r="A31" s="3">
+        <v>830119707</v>
+      </c>
     </row>
     <row r="32" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="4"/>
+      <c r="A32" s="3">
+        <v>860404520</v>
+      </c>
     </row>
     <row r="33" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="4"/>
+      <c r="A33" s="3">
+        <v>860450841</v>
+      </c>
     </row>
     <row r="34" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="4"/>
+      <c r="A34" s="3">
+        <v>900473941</v>
+      </c>
     </row>
     <row r="35" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="4"/>
+      <c r="A35" s="3">
+        <v>900404487</v>
+      </c>
     </row>
     <row r="36" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="4"/>
+      <c r="A36" s="3">
+        <v>830131333</v>
+      </c>
     </row>
     <row r="37" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="4"/>
+      <c r="A37" s="3">
+        <v>900098431</v>
+      </c>
     </row>
     <row r="38" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="4"/>
+      <c r="A38" s="3">
+        <v>900521142</v>
+      </c>
     </row>
     <row r="39" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="4"/>
+      <c r="A39" s="3">
+        <v>830123384</v>
+      </c>
     </row>
     <row r="40" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="4"/>
+      <c r="A40" s="3">
+        <v>832005276</v>
+      </c>
     </row>
     <row r="41" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="4"/>
+      <c r="A41" s="3">
+        <v>900060600</v>
+      </c>
     </row>
     <row r="42" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="4"/>
+      <c r="A42" s="3">
+        <v>830116263</v>
+      </c>
     </row>
     <row r="43" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="4"/>
+      <c r="A43" s="3">
+        <v>900545280</v>
+      </c>
     </row>
     <row r="44" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="4"/>
+      <c r="A44" s="3">
+        <v>900334680</v>
+      </c>
     </row>
     <row r="45" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="4"/>
+      <c r="A45" s="3">
+        <v>900208664</v>
+      </c>
     </row>
     <row r="46" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="4"/>
+      <c r="A46" s="3">
+        <v>900715424</v>
+      </c>
     </row>
     <row r="47" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="4"/>
+      <c r="A47" s="3">
+        <v>901151343</v>
+      </c>
     </row>
     <row r="48" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="4"/>
+      <c r="A48" s="3">
+        <v>900271099</v>
+      </c>
     </row>
     <row r="49" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="4"/>
+      <c r="A49" s="3">
+        <v>900194299</v>
+      </c>
     </row>
     <row r="50" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="4"/>
+      <c r="A50" s="3">
+        <v>900539381</v>
+      </c>
     </row>
     <row r="51" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="4"/>
+      <c r="A51" s="3">
+        <v>830133314</v>
+      </c>
     </row>
     <row r="52" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="4"/>
+      <c r="A52" s="3">
+        <v>900748799</v>
+      </c>
     </row>
     <row r="53" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="4"/>
+      <c r="A53" s="3">
+        <v>9003223880</v>
+      </c>
     </row>
     <row r="54" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="4"/>
-    </row>
-    <row r="55" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A55"/>
-    </row>
-    <row r="56" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A56"/>
-    </row>
-    <row r="57" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A57"/>
-    </row>
-    <row r="58" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A58"/>
-    </row>
-    <row r="59" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A59"/>
-    </row>
-    <row r="60" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A60"/>
-    </row>
-    <row r="61" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A61"/>
-    </row>
-    <row r="62" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A62"/>
-    </row>
-    <row r="63" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A63"/>
-    </row>
-    <row r="64" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A64"/>
-    </row>
-    <row r="65" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A65"/>
-    </row>
-    <row r="66" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A66"/>
-    </row>
-    <row r="67" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A67"/>
-    </row>
-    <row r="68" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A68"/>
-    </row>
-    <row r="69" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A69"/>
-    </row>
-    <row r="70" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A70"/>
-    </row>
-    <row r="71" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A71"/>
-    </row>
-    <row r="72" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A72"/>
-    </row>
-    <row r="73" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A73"/>
-    </row>
-    <row r="74" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A74"/>
-    </row>
-    <row r="75" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A75"/>
-    </row>
-    <row r="76" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A76"/>
-    </row>
-    <row r="77" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A77"/>
-    </row>
-    <row r="78" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A78"/>
-    </row>
-    <row r="79" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A79"/>
-    </row>
-    <row r="80" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A80"/>
-    </row>
-    <row r="81" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A81"/>
-    </row>
-    <row r="82" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A82"/>
-    </row>
-    <row r="83" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A83"/>
-    </row>
-    <row r="84" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A84"/>
-    </row>
-    <row r="85" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A85"/>
-    </row>
-    <row r="86" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A86"/>
-    </row>
-    <row r="87" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A87"/>
-    </row>
-    <row r="88" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A88"/>
-    </row>
-    <row r="89" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A89"/>
-    </row>
-    <row r="90" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A90"/>
-    </row>
-    <row r="91" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A91"/>
-    </row>
-    <row r="92" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A92"/>
-    </row>
-    <row r="93" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A93"/>
-    </row>
-    <row r="94" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A94"/>
-    </row>
-    <row r="95" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A95"/>
-    </row>
-    <row r="96" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A96"/>
-    </row>
-    <row r="97" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A97"/>
-    </row>
-    <row r="98" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A98"/>
-    </row>
-    <row r="99" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A99"/>
-    </row>
-    <row r="100" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A100"/>
-    </row>
-    <row r="101" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A101"/>
-    </row>
-    <row r="102" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A102"/>
-    </row>
-    <row r="103" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A103"/>
-    </row>
-    <row r="104" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A104"/>
-    </row>
-    <row r="105" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A105"/>
-    </row>
-    <row r="106" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A106"/>
-    </row>
-    <row r="107" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A107"/>
+      <c r="A54" s="3">
+        <v>900643491</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="3">
+        <v>900247733</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="3">
+        <v>900546980</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="3">
+        <v>900489785</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="3">
+        <v>860100007</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="3">
+        <v>900379513</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="3">
+        <v>901509798</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A107">
-    <sortCondition ref="A1:A107"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A12">
+    <sortCondition ref="A1:A12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajuste de migracion de clientes y procesos judiciales
</commit_message>
<xml_diff>
--- a/migracion/migracionXnit.xlsx
+++ b/migracion/migracionXnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\DesarrolloWeb358\gestion-global\migracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7A137A-AF06-4966-BE0C-C71F14336C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6DC2D3-F276-4942-9E6C-EC165E341157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{23831529-313D-4FD4-9556-5C5894147868}"/>
   </bookViews>
@@ -56,18 +56,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -97,11 +91,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -418,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57688D05-55A1-47BC-8BE5-91F4BB88B5A9}">
-  <dimension ref="A1:A60"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
@@ -431,309 +424,81 @@
     <col min="3" max="3" width="30.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
-        <v>830035457</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
+        <v>830036121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
-        <v>830047278</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
+        <v>900051936</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
-        <v>830057747</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
+        <v>900745947</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
-        <v>830071809</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
+        <v>830105124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
-        <v>830074497</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>900143246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
-        <v>830075332</v>
+        <v>900176157</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="3">
-        <v>900687420</v>
+      <c r="A8" s="2">
+        <v>900026123</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="3">
-        <v>900346849</v>
+      <c r="A9" s="2">
+        <v>900754972</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="3">
-        <v>900281120</v>
+      <c r="A10" s="2">
+        <v>900040178</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="3">
-        <v>900003261</v>
+      <c r="A11" s="2">
+        <v>900162919</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="3">
-        <v>900947384</v>
+      <c r="A12" s="2">
+        <v>900153423</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="3">
-        <v>901507077</v>
-      </c>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="3">
-        <v>900719501</v>
-      </c>
+      <c r="A14" s="2"/>
     </row>
     <row r="15" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="3">
-        <v>900658412</v>
-      </c>
+      <c r="A15" s="2"/>
     </row>
     <row r="16" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="3">
-        <v>900182882</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="3">
-        <v>900061167</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="3">
-        <v>901001861</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="3">
-        <v>900123743</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="3">
-        <v>900377532</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="3">
-        <v>900190116</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="3">
-        <v>900155802</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="3">
-        <v>900506434</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="3">
-        <v>830121765</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="3">
-        <v>900122253</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="3">
-        <v>830096405</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="3">
-        <v>860040335</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="3">
-        <v>901194167</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="3">
-        <v>901132823</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="3">
-        <v>830125131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="3">
-        <v>830119707</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="3">
-        <v>860404520</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="3">
-        <v>860450841</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="3">
-        <v>900473941</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="3">
-        <v>900404487</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="3">
-        <v>830131333</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="3">
-        <v>900098431</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="3">
-        <v>900521142</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="3">
-        <v>830123384</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="3">
-        <v>832005276</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="3">
-        <v>900060600</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="3">
-        <v>830116263</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="3">
-        <v>900545280</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="3">
-        <v>900334680</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="3">
-        <v>900208664</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="3">
-        <v>900715424</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="3">
-        <v>901151343</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="3">
-        <v>900271099</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="3">
-        <v>900194299</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="3">
-        <v>900539381</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="3">
-        <v>830133314</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="3">
-        <v>900748799</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="3">
-        <v>9003223880</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="3">
-        <v>900643491</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="3">
-        <v>900247733</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="3">
-        <v>900546980</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="3">
-        <v>900489785</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="3">
-        <v>860100007</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="3">
-        <v>900379513</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="3">
-        <v>901509798</v>
-      </c>
+      <c r="A16" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A12">
-    <sortCondition ref="A1:A12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A10">
+    <sortCondition ref="A1:A10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ajuste migracion seguimiento y pantalla
</commit_message>
<xml_diff>
--- a/migracion/migracionXnit.xlsx
+++ b/migracion/migracionXnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\DesarrolloWeb358\gestion-global\migracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED18867-E778-4F57-9438-7598CF82F36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A026B3-1A60-4457-B72A-989ADB9B0FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{23831529-313D-4FD4-9556-5C5894147868}"/>
   </bookViews>
@@ -56,18 +56,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -100,7 +94,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -417,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57688D05-55A1-47BC-8BE5-91F4BB88B5A9}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
@@ -437,7 +431,52 @@
     </row>
     <row r="2" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
-        <v>900495255</v>
+        <v>900687420</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2">
+        <v>900291664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2">
+        <v>830018673</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="2">
+        <v>900387627</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="2">
+        <v>900123743</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2">
+        <v>901001861</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="2">
+        <v>900003261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="2">
+        <v>900377532</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="2">
+        <v>900190116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="2">
+        <v>900155802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajuste migracion ejecutivos vacios
</commit_message>
<xml_diff>
--- a/migracion/migracionXnit.xlsx
+++ b/migracion/migracionXnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\DesarrolloWeb358\gestion-global\migracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A026B3-1A60-4457-B72A-989ADB9B0FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFA022F-3871-4F71-9B58-FA07352275AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{23831529-313D-4FD4-9556-5C5894147868}"/>
   </bookViews>
@@ -56,12 +56,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -91,10 +97,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -411,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57688D05-55A1-47BC-8BE5-91F4BB88B5A9}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
@@ -430,53 +439,103 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>900687420</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>900291664</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>830018673</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>900387627</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>900123743</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="2">
+      <c r="A7" s="3">
         <v>901001861</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="2">
+      <c r="A8" s="3">
         <v>900003261</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="2">
+      <c r="A9" s="3">
         <v>900377532</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>900190116</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <v>900155802</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="2">
+        <v>900506434</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="2">
+        <v>900654612</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="2">
+        <v>830032420</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="2">
+        <v>900715424</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="2">
+        <v>830006055</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="2">
+        <v>900947384</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="2">
+        <v>830125131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="2">
+        <v>830121765</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="2">
+        <v>800142993</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="2">
+        <v>830074497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajuste reporte estados mensuales
</commit_message>
<xml_diff>
--- a/migracion/migracionXnit.xlsx
+++ b/migracion/migracionXnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\DesarrolloWeb358\gestion-global\migracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFA022F-3871-4F71-9B58-FA07352275AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833AEC9F-BEC2-4DB0-847B-1B484F486C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{23831529-313D-4FD4-9556-5C5894147868}"/>
   </bookViews>
@@ -56,18 +56,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -97,13 +91,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -422,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57688D05-55A1-47BC-8BE5-91F4BB88B5A9}">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
@@ -439,104 +430,84 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3">
-        <v>900687420</v>
+      <c r="A2" s="2">
+        <v>800057394</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="3">
-        <v>900291664</v>
+      <c r="A3" s="2">
+        <v>900849952</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3">
-        <v>830018673</v>
+      <c r="A4" s="2">
+        <v>830074930</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="3">
-        <v>900387627</v>
+      <c r="A5" s="2">
+        <v>800238184</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="3">
-        <v>900123743</v>
+      <c r="A6" s="2">
+        <v>830071086</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="3">
-        <v>901001861</v>
+      <c r="A7" s="2">
+        <v>900051936</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="3">
-        <v>900003261</v>
+      <c r="A8" s="2">
+        <v>860530921</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="3">
-        <v>900377532</v>
+      <c r="A9" s="2">
+        <v>900745947</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="3">
-        <v>900190116</v>
+      <c r="A10" s="2">
+        <v>900323880</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="3">
-        <v>900155802</v>
+      <c r="A11" s="2">
+        <v>900643491</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="2">
-        <v>900506434</v>
-      </c>
+      <c r="A12" s="2"/>
     </row>
     <row r="13" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2">
-        <v>900654612</v>
-      </c>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="2">
-        <v>830032420</v>
-      </c>
+      <c r="A14" s="2"/>
     </row>
     <row r="15" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="2">
-        <v>900715424</v>
-      </c>
+      <c r="A15" s="2"/>
     </row>
     <row r="16" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="2">
-        <v>830006055</v>
-      </c>
+      <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="2">
-        <v>900947384</v>
-      </c>
+      <c r="A17" s="2"/>
     </row>
     <row r="18" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="2">
-        <v>830125131</v>
-      </c>
+      <c r="A18" s="2"/>
     </row>
     <row r="19" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="2">
-        <v>830121765</v>
-      </c>
+      <c r="A19" s="2"/>
     </row>
     <row r="20" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="2">
-        <v>800142993</v>
-      </c>
+      <c r="A20" s="2"/>
     </row>
     <row r="21" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="2">
-        <v>830074497</v>
-      </c>
+      <c r="A21" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2">

</xml_diff>

<commit_message>
ajustes diseño y  migracion
</commit_message>
<xml_diff>
--- a/migracion/migracionXnit.xlsx
+++ b/migracion/migracionXnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\DesarrolloWeb358\gestion-global\migracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833AEC9F-BEC2-4DB0-847B-1B484F486C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7809708-516B-4DC7-91B5-A1AEB15F9189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{23831529-313D-4FD4-9556-5C5894147868}"/>
   </bookViews>
@@ -56,12 +56,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -94,7 +100,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -411,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57688D05-55A1-47BC-8BE5-91F4BB88B5A9}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="A176" sqref="A176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
@@ -431,83 +437,878 @@
     </row>
     <row r="2" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
-        <v>800057394</v>
+        <v>900687420</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
-        <v>900849952</v>
+        <v>900291664</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
-        <v>830074930</v>
+        <v>830018673</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
-        <v>800238184</v>
+        <v>900387627</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
-        <v>830071086</v>
+        <v>900123743</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
-        <v>900051936</v>
+        <v>901001861</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2">
-        <v>860530921</v>
+        <v>900003261</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
-        <v>900745947</v>
+        <v>900377532</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2">
-        <v>900323880</v>
+        <v>900190116</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2">
+        <v>900155802</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="2">
+        <v>900506434</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="2">
+        <v>900654612</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="2">
+        <v>830032420</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="2">
+        <v>900715424</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="2">
+        <v>830006055</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="2">
+        <v>900947384</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="2">
+        <v>830125131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="2">
+        <v>830121765</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="2">
+        <v>800142993</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="2">
+        <v>830074497</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2">
+        <v>900122253</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2">
+        <v>800119310</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="2">
+        <v>830057747</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="2">
+        <v>900658412</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="2">
+        <v>900281120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="2">
+        <v>830096405</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="2">
+        <v>900539381</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="2">
+        <v>900266721</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="2">
+        <v>900366498</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="2">
+        <v>860040335</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="2">
+        <v>900786792</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="2">
+        <v>830064945</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="2">
+        <v>901507077</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="2">
+        <v>901132823</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2">
+        <v>901213216</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="2">
+        <v>800193176</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="2">
+        <v>830075332</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="2">
+        <v>800206093</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="2">
+        <v>830135812</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="2">
+        <v>832005276</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="2">
+        <v>800234376</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="2">
+        <v>860404520</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="2">
+        <v>830113468</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="2">
+        <v>800177027</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="2">
+        <v>830119707</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="2">
+        <v>800237079</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="2">
+        <v>900473941</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="2">
+        <v>860450841</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="2">
+        <v>900060600</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="2">
+        <v>900404487</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="2">
+        <v>900084381</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="2">
+        <v>830131333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="2">
+        <v>900182882</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="2">
+        <v>901554013</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="2">
+        <v>830113211</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="2">
+        <v>830076458</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="2">
+        <v>900759684</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="2">
+        <v>901747169</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="2">
+        <v>900121375</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="2">
+        <v>900328260</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="2">
+        <v>900232631</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="2">
+        <v>900481528</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="2">
+        <v>901562955</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="2">
+        <v>900237253</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="2">
+        <v>860352766</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="2">
+        <v>800095818</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="2">
+        <v>830088870</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="2">
+        <v>900334680</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="2">
+        <v>900715763</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="2">
+        <v>900495255</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="2">
+        <v>830146081</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="2">
+        <v>900367986</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="2">
+        <v>800250273</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A75" s="2">
+        <v>830027772</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="2">
+        <v>900229811</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="2">
+        <v>900719591</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="2">
+        <v>900748799</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="2">
+        <v>900115005</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="2">
+        <v>830079494</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="2">
+        <v>809011754</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="2">
+        <v>830002180</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="2">
+        <v>800198168</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="2">
+        <v>900947320</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="2">
+        <v>900346849</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="2">
+        <v>830115545</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="2">
+        <v>901335235</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="2">
+        <v>900812356</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="2">
+        <v>900042174</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="2">
+        <v>901332807</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="2">
+        <v>901031409</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="2">
+        <v>901400806</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="2">
+        <v>830036121</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="2">
+        <v>800057394</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A95" s="2">
+        <v>900849952</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="2">
+        <v>830074930</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A97" s="2">
+        <v>800238184</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="2">
+        <v>830071086</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A99" s="2">
+        <v>900051936</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A100" s="2">
+        <v>860530921</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="2">
+        <v>900745947</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A102" s="2">
+        <v>900323880</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A103" s="2">
         <v>900643491</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="2"/>
+    <row r="104" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A104" s="2">
+        <v>901359839</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A105" s="2">
+        <v>900422149</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="2">
+        <v>830077961</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="2">
+        <v>830073688</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A108" s="2">
+        <v>900253555</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="2">
+        <v>900296386</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="2">
+        <v>900305611</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="2">
+        <v>900143246</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A112" s="2">
+        <v>830105124</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A113" s="2">
+        <v>830042740</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A114" s="2">
+        <v>830013285</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A115" s="2">
+        <v>800217483</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A116" s="2">
+        <v>830015808</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A117" s="2">
+        <v>900208664</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A118" s="2">
+        <v>901194167</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A119" s="2">
+        <v>900176157</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A120" s="2">
+        <v>900123118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A121" s="2">
+        <v>830116263</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A122" s="2">
+        <v>900242902</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A123" s="2">
+        <v>900247733</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A124" s="2">
+        <v>830035457</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A125" s="2">
+        <v>900026123</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A126" s="2">
+        <v>900754972</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A127" s="2">
+        <v>830094327</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A128" s="2">
+        <v>900040178</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A129" s="2">
+        <v>900162919</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A130" s="2">
+        <v>900153423</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A131" s="2">
+        <v>900546980</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A132" s="2">
+        <v>800190771</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A133" s="2">
+        <v>901334383</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A134" s="2">
+        <v>800168829</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A135" s="2">
+        <v>900271099</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A136" s="2">
+        <v>800236456</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A137" s="2">
+        <v>900361188</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A138" s="2">
+        <v>900353436</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A139" s="2">
+        <v>901268833</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A140" s="2">
+        <v>900002446</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A141" s="2">
+        <v>830047278</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A142" s="2">
+        <v>900097482</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A143" s="2">
+        <v>830056841</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A144" s="2">
+        <v>900243855</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A145" s="2">
+        <v>830032560</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A146" s="2">
+        <v>830147668</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A147" s="2">
+        <v>900863645</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A148" s="2">
+        <v>900840280</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A149" s="2">
+        <v>900382589</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A150" s="2">
+        <v>900489785</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A151" s="2">
+        <v>900360842</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A152" s="2">
+        <v>860100007</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A153" s="2">
+        <v>830042712</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A154" s="2">
+        <v>800115495</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A155" s="2">
+        <v>900545280</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A156" s="2">
+        <v>901020816</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A157" s="2">
+        <v>900273325</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A158" s="2">
+        <v>900283218</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A159" s="2">
+        <v>901801045</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A160" s="2">
+        <v>830018187</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A161" s="2">
+        <v>900061167</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A162" s="2">
+        <v>900194299</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A163" s="2">
+        <v>830147484</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A164" s="2">
+        <v>901151343</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A165" s="2">
+        <v>860043705</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A166" s="2">
+        <v>901458746</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A167" s="2">
+        <v>830089370</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A168" s="2">
+        <v>830102273</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A169" s="2">
+        <v>900309487</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A170" s="2">
+        <v>900227246</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A171" s="2">
+        <v>900306295</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A172" s="2">
+        <v>900041729</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A173" s="2">
+        <v>830136067</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A174" s="2">
+        <v>900746489</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A175" s="2">
+        <v>901509798</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A176" s="2">
+        <v>900892217</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2">

</xml_diff>

<commit_message>
roles y permisos para cargar los clientes
</commit_message>
<xml_diff>
--- a/migracion/migracionXnit.xlsx
+++ b/migracion/migracionXnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\DesarrolloWeb358\gestion-global\migracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31F50EB-080E-4FF4-84BA-8352A5C2777F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41096E40-4224-402E-B302-1C0862112A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{23831529-313D-4FD4-9556-5C5894147868}"/>
   </bookViews>
@@ -25,76 +25,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>nit</t>
-  </si>
-  <si>
-    <t>900291664</t>
-  </si>
-  <si>
-    <t>830015808</t>
-  </si>
-  <si>
-    <t>900153423</t>
-  </si>
-  <si>
-    <t>900539381</t>
-  </si>
-  <si>
-    <t>901359839</t>
-  </si>
-  <si>
-    <t>900026123</t>
-  </si>
-  <si>
-    <t>901507077</t>
-  </si>
-  <si>
-    <t>830056841</t>
-  </si>
-  <si>
-    <t>900654612</t>
-  </si>
-  <si>
-    <t>830074930</t>
-  </si>
-  <si>
-    <t>900123118</t>
-  </si>
-  <si>
-    <t>900041729</t>
-  </si>
-  <si>
-    <t>900194299</t>
-  </si>
-  <si>
-    <t>900051936</t>
-  </si>
-  <si>
-    <t>900422149</t>
-  </si>
-  <si>
-    <t>800237079</t>
-  </si>
-  <si>
-    <t>830042740</t>
-  </si>
-  <si>
-    <t>900367986</t>
-  </si>
-  <si>
-    <t>900182882</t>
-  </si>
-  <si>
-    <t>830113468</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +51,14 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -137,12 +85,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57688D05-55A1-47BC-8BE5-91F4BB88B5A9}">
-  <dimension ref="A1:A44"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
@@ -470,225 +419,136 @@
     <col min="3" max="3" width="30.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>830015808</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A2" s="1">
+        <v>900654612</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
-        <v>830074930</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>830042740</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>900291664</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>900367986</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>900153423</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>900060600</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
-        <v>900123118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
-        <v>900754972</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
-        <v>901359839</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
-        <v>900041729</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
-        <v>900194299</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
-        <v>900051936</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
-        <v>901507077</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
-        <v>900422149</v>
-      </c>
+    <row r="5" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
-        <v>900182882</v>
-      </c>
+      <c r="A17" s="2"/>
     </row>
     <row r="18" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
-        <v>900026123</v>
-      </c>
+      <c r="A18" s="2"/>
     </row>
     <row r="19" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
-        <v>900539381</v>
-      </c>
+      <c r="A19" s="2"/>
     </row>
     <row r="20" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
-        <v>901001861</v>
-      </c>
+      <c r="A20" s="2"/>
     </row>
     <row r="21" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
-        <v>830113468</v>
-      </c>
+      <c r="A21" s="2"/>
     </row>
     <row r="22" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
-        <v>800237079</v>
-      </c>
+      <c r="A22" s="2"/>
     </row>
     <row r="23" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
-        <v>830056841</v>
-      </c>
+      <c r="A23" s="2"/>
     </row>
     <row r="24" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="A24" s="2"/>
     </row>
     <row r="25" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A25" s="2"/>
     </row>
     <row r="26" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A26" s="2"/>
     </row>
     <row r="27" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A27" s="2"/>
     </row>
     <row r="28" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="A28" s="2"/>
     </row>
     <row r="29" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A29" s="2"/>
     </row>
     <row r="30" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A30" s="2"/>
     </row>
     <row r="31" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A31" s="2"/>
     </row>
     <row r="32" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A32" s="2"/>
     </row>
     <row r="33" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A33" s="2"/>
     </row>
     <row r="34" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A34" s="2"/>
     </row>
     <row r="35" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A35" s="2"/>
     </row>
     <row r="36" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="A36" s="2"/>
     </row>
     <row r="37" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A37" s="2"/>
     </row>
     <row r="38" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A38" s="2"/>
     </row>
     <row r="39" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="A39" s="2"/>
     </row>
     <row r="40" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A40" s="2"/>
     </row>
     <row r="41" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="A41" s="2"/>
     </row>
     <row r="42" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A42" s="2"/>
     </row>
     <row r="43" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A43" s="2"/>
     </row>
     <row r="44" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="2">
-        <v>800245235</v>
-      </c>
+      <c r="A44" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>